<commit_message>
Update redirects file for redirection of the history.html file
This is to ensure that the build.fhir publish box link for 'directory of published versions redirects to the correct endpoint in fhir.digitalhealth.gov.au
</commit_message>
<xml_diff>
--- a/ADHA-FHIR-IG-redirects.xlsx
+++ b/ADHA-FHIR-IG-redirects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\ci-fhir-r4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15CAA72-9A8A-4AAC-9F1D-749BC12CECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8B8844-D142-4A19-9DC0-4DBB2DF56FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="2595" windowWidth="27360" windowHeight="11310" xr2:uid="{809266FD-E24E-4962-B240-F4A51F3B0C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{809266FD-E24E-4962-B240-F4A51F3B0C12}"/>
   </bookViews>
   <sheets>
     <sheet name="Publication redirects" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Australian Digital Health Agency FHIR Implementation Guide v1.0.0</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>https://fhir.digitalhealth.gov.au/dh/package.tgz</t>
+  </si>
+  <si>
+    <t>http://ns.electronichealth.net.au/fhir/history.html</t>
+  </si>
+  <si>
+    <t>https://fhir.digitalhealth.gov.au/dh/history.html</t>
   </si>
 </sst>
 </file>
@@ -660,16 +666,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11248DB4-03C3-48B9-8F87-76A85990C6DC}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,6 +745,14 @@
       </c>
       <c r="B11" s="2" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -755,9 +769,11 @@
     <hyperlink ref="B10" r:id="rId10" xr:uid="{E1572E35-F24B-4DFE-95A8-99E52FC35FD9}"/>
     <hyperlink ref="A11" r:id="rId11" xr:uid="{AFDF7123-1CD3-4C93-9EDF-57144697825D}"/>
     <hyperlink ref="B11" r:id="rId12" xr:uid="{AD1D58BC-7C70-4DD4-A2BD-CB0A8F8F0FBD}"/>
+    <hyperlink ref="A12" r:id="rId13" xr:uid="{3C82DAEA-5345-4596-A2D3-12336C269DB2}"/>
+    <hyperlink ref="B12" r:id="rId14" xr:uid="{0DE2AA09-53C0-4729-BAB3-BCCB19156531}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>